<commit_message>
Cleaning and EDA update
</commit_message>
<xml_diff>
--- a/Data_of_Interest_Cleaned/minimum_wage_global_interest.xlsx
+++ b/Data_of_Interest_Cleaned/minimum_wage_global_interest.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D266"/>
+  <dimension ref="A1:D343"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3392,7 +3392,7 @@
     <row r="165">
       <c r="A165" t="inlineStr">
         <is>
-          <t>Myanmar</t>
+          <t>South Korea</t>
         </is>
       </c>
       <c r="B165" t="inlineStr">
@@ -3401,16 +3401,16 @@
         </is>
       </c>
       <c r="C165" t="n">
-        <v>2020</v>
+        <v>2023</v>
       </c>
       <c r="D165" t="n">
-        <v>90.32899999999999</v>
+        <v>1539.893</v>
       </c>
     </row>
     <row r="166">
       <c r="A166" t="inlineStr">
         <is>
-          <t>Myanmar</t>
+          <t>South Korea</t>
         </is>
       </c>
       <c r="B166" t="inlineStr">
@@ -3419,16 +3419,16 @@
         </is>
       </c>
       <c r="C166" t="n">
-        <v>2019</v>
+        <v>2022</v>
       </c>
       <c r="D166" t="n">
-        <v>82.2</v>
+        <v>1482.4</v>
       </c>
     </row>
     <row r="167">
       <c r="A167" t="inlineStr">
         <is>
-          <t>Myanmar</t>
+          <t>South Korea</t>
         </is>
       </c>
       <c r="B167" t="inlineStr">
@@ -3437,16 +3437,16 @@
         </is>
       </c>
       <c r="C167" t="n">
-        <v>2018</v>
+        <v>2021</v>
       </c>
       <c r="D167" t="n">
-        <v>87.28400000000001</v>
+        <v>1593.144</v>
       </c>
     </row>
     <row r="168">
       <c r="A168" t="inlineStr">
         <is>
-          <t>Myanmar</t>
+          <t>South Korea</t>
         </is>
       </c>
       <c r="B168" t="inlineStr">
@@ -3455,16 +3455,16 @@
         </is>
       </c>
       <c r="C168" t="n">
-        <v>2017</v>
+        <v>2020</v>
       </c>
       <c r="D168" t="n">
-        <v>68.80500000000001</v>
+        <v>1521.107</v>
       </c>
     </row>
     <row r="169">
       <c r="A169" t="inlineStr">
         <is>
-          <t>Myanmar</t>
+          <t>South Korea</t>
         </is>
       </c>
       <c r="B169" t="inlineStr">
@@ -3473,16 +3473,16 @@
         </is>
       </c>
       <c r="C169" t="n">
-        <v>2016</v>
+        <v>2019</v>
       </c>
       <c r="D169" t="n">
-        <v>75.798</v>
+        <v>1497.523</v>
       </c>
     </row>
     <row r="170">
       <c r="A170" t="inlineStr">
         <is>
-          <t>Myanmar</t>
+          <t>South Korea</t>
         </is>
       </c>
       <c r="B170" t="inlineStr">
@@ -3491,16 +3491,16 @@
         </is>
       </c>
       <c r="C170" t="n">
-        <v>2015</v>
+        <v>2018</v>
       </c>
       <c r="D170" t="n">
-        <v>80.508</v>
+        <v>1430.488</v>
       </c>
     </row>
     <row r="171">
       <c r="A171" t="inlineStr">
         <is>
-          <t>Malaysia</t>
+          <t>South Korea</t>
         </is>
       </c>
       <c r="B171" t="inlineStr">
@@ -3509,16 +3509,16 @@
         </is>
       </c>
       <c r="C171" t="n">
-        <v>2023</v>
+        <v>2017</v>
       </c>
       <c r="D171" t="n">
-        <v>328.902</v>
+        <v>1195.605</v>
       </c>
     </row>
     <row r="172">
       <c r="A172" t="inlineStr">
         <is>
-          <t>Malaysia</t>
+          <t>South Korea</t>
         </is>
       </c>
       <c r="B172" t="inlineStr">
@@ -3527,16 +3527,16 @@
         </is>
       </c>
       <c r="C172" t="n">
-        <v>2022</v>
+        <v>2016</v>
       </c>
       <c r="D172" t="n">
-        <v>340.826</v>
+        <v>1085.721</v>
       </c>
     </row>
     <row r="173">
       <c r="A173" t="inlineStr">
         <is>
-          <t>Malaysia</t>
+          <t>South Korea</t>
         </is>
       </c>
       <c r="B173" t="inlineStr">
@@ -3545,16 +3545,16 @@
         </is>
       </c>
       <c r="C173" t="n">
-        <v>2021</v>
+        <v>2015</v>
       </c>
       <c r="D173" t="n">
-        <v>289.624</v>
+        <v>1031.184</v>
       </c>
     </row>
     <row r="174">
       <c r="A174" t="inlineStr">
         <is>
-          <t>Malaysia</t>
+          <t>South Korea</t>
         </is>
       </c>
       <c r="B174" t="inlineStr">
@@ -3563,16 +3563,16 @@
         </is>
       </c>
       <c r="C174" t="n">
-        <v>2020</v>
+        <v>2014</v>
       </c>
       <c r="D174" t="n">
-        <v>285.478</v>
+        <v>1034.241</v>
       </c>
     </row>
     <row r="175">
       <c r="A175" t="inlineStr">
         <is>
-          <t>Malaysia</t>
+          <t>South Korea</t>
         </is>
       </c>
       <c r="B175" t="inlineStr">
@@ -3581,16 +3581,16 @@
         </is>
       </c>
       <c r="C175" t="n">
-        <v>2019</v>
+        <v>2013</v>
       </c>
       <c r="D175" t="n">
-        <v>265.542</v>
+        <v>927.631</v>
       </c>
     </row>
     <row r="176">
       <c r="A176" t="inlineStr">
         <is>
-          <t>Malaysia</t>
+          <t>South Korea</t>
         </is>
       </c>
       <c r="B176" t="inlineStr">
@@ -3599,16 +3599,16 @@
         </is>
       </c>
       <c r="C176" t="n">
-        <v>2018</v>
+        <v>2012</v>
       </c>
       <c r="D176" t="n">
-        <v>247.823</v>
+        <v>849.498</v>
       </c>
     </row>
     <row r="177">
       <c r="A177" t="inlineStr">
         <is>
-          <t>Malaysia</t>
+          <t>South Korea</t>
         </is>
       </c>
       <c r="B177" t="inlineStr">
@@ -3617,16 +3617,16 @@
         </is>
       </c>
       <c r="C177" t="n">
-        <v>2017</v>
+        <v>2011</v>
       </c>
       <c r="D177" t="n">
-        <v>232.534</v>
+        <v>814.702</v>
       </c>
     </row>
     <row r="178">
       <c r="A178" t="inlineStr">
         <is>
-          <t>Malaysia</t>
+          <t>South Korea</t>
         </is>
       </c>
       <c r="B178" t="inlineStr">
@@ -3635,16 +3635,16 @@
         </is>
       </c>
       <c r="C178" t="n">
-        <v>2016</v>
+        <v>2010</v>
       </c>
       <c r="D178" t="n">
-        <v>241.063</v>
+        <v>803.192</v>
       </c>
     </row>
     <row r="179">
       <c r="A179" t="inlineStr">
         <is>
-          <t>Malaysia</t>
+          <t>South Korea</t>
         </is>
       </c>
       <c r="B179" t="inlineStr">
@@ -3653,16 +3653,16 @@
         </is>
       </c>
       <c r="C179" t="n">
-        <v>2015</v>
+        <v>2009</v>
       </c>
       <c r="D179" t="n">
-        <v>230.444</v>
+        <v>707.773</v>
       </c>
     </row>
     <row r="180">
       <c r="A180" t="inlineStr">
         <is>
-          <t>Malaysia</t>
+          <t>South Korea</t>
         </is>
       </c>
       <c r="B180" t="inlineStr">
@@ -3671,16 +3671,16 @@
         </is>
       </c>
       <c r="C180" t="n">
-        <v>2014</v>
+        <v>2008</v>
       </c>
       <c r="D180" t="n">
-        <v>274.989</v>
+        <v>774.475</v>
       </c>
     </row>
     <row r="181">
       <c r="A181" t="inlineStr">
         <is>
-          <t>Malaysia</t>
+          <t>South Korea</t>
         </is>
       </c>
       <c r="B181" t="inlineStr">
@@ -3689,16 +3689,16 @@
         </is>
       </c>
       <c r="C181" t="n">
-        <v>2013</v>
+        <v>2007</v>
       </c>
       <c r="D181" t="n">
-        <v>285.632</v>
+        <v>846.245</v>
       </c>
     </row>
     <row r="182">
       <c r="A182" t="inlineStr">
         <is>
-          <t>New Zealand</t>
+          <t>South Korea</t>
         </is>
       </c>
       <c r="B182" t="inlineStr">
@@ -3707,16 +3707,16 @@
         </is>
       </c>
       <c r="C182" t="n">
-        <v>2023</v>
+        <v>2006</v>
       </c>
       <c r="D182" t="n">
-        <v>2414.37</v>
+        <v>733.351</v>
       </c>
     </row>
     <row r="183">
       <c r="A183" t="inlineStr">
         <is>
-          <t>New Zealand</t>
+          <t>South Korea</t>
         </is>
       </c>
       <c r="B183" t="inlineStr">
@@ -3725,16 +3725,16 @@
         </is>
       </c>
       <c r="C183" t="n">
-        <v>2022</v>
+        <v>2005</v>
       </c>
       <c r="D183" t="n">
-        <v>2329.892</v>
+        <v>626.596</v>
       </c>
     </row>
     <row r="184">
       <c r="A184" t="inlineStr">
         <is>
-          <t>New Zealand</t>
+          <t>South Korea</t>
         </is>
       </c>
       <c r="B184" t="inlineStr">
@@ -3743,16 +3743,16 @@
         </is>
       </c>
       <c r="C184" t="n">
-        <v>2021</v>
+        <v>2004</v>
       </c>
       <c r="D184" t="n">
-        <v>2452.021</v>
+        <v>494.884</v>
       </c>
     </row>
     <row r="185">
       <c r="A185" t="inlineStr">
         <is>
-          <t>New Zealand</t>
+          <t>South Korea</t>
         </is>
       </c>
       <c r="B185" t="inlineStr">
@@ -3761,16 +3761,16 @@
         </is>
       </c>
       <c r="C185" t="n">
-        <v>2020</v>
+        <v>2003</v>
       </c>
       <c r="D185" t="n">
-        <v>2124.433</v>
+        <v>431.462</v>
       </c>
     </row>
     <row r="186">
       <c r="A186" t="inlineStr">
         <is>
-          <t>New Zealand</t>
+          <t>South Korea</t>
         </is>
       </c>
       <c r="B186" t="inlineStr">
@@ -3779,16 +3779,16 @@
         </is>
       </c>
       <c r="C186" t="n">
-        <v>2019</v>
+        <v>2002</v>
       </c>
       <c r="D186" t="n">
-        <v>2021.247</v>
+        <v>379.194</v>
       </c>
     </row>
     <row r="187">
       <c r="A187" t="inlineStr">
         <is>
-          <t>New Zealand</t>
+          <t>South Korea</t>
         </is>
       </c>
       <c r="B187" t="inlineStr">
@@ -3797,16 +3797,16 @@
         </is>
       </c>
       <c r="C187" t="n">
-        <v>2018</v>
+        <v>2001</v>
       </c>
       <c r="D187" t="n">
-        <v>1978.885</v>
+        <v>326.536</v>
       </c>
     </row>
     <row r="188">
       <c r="A188" t="inlineStr">
         <is>
-          <t>New Zealand</t>
+          <t>South Korea</t>
         </is>
       </c>
       <c r="B188" t="inlineStr">
@@ -3815,16 +3815,16 @@
         </is>
       </c>
       <c r="C188" t="n">
-        <v>2017</v>
+        <v>2000</v>
       </c>
       <c r="D188" t="n">
-        <v>1939.736</v>
+        <v>319.897</v>
       </c>
     </row>
     <row r="189">
       <c r="A189" t="inlineStr">
         <is>
-          <t>New Zealand</t>
+          <t>South Korea</t>
         </is>
       </c>
       <c r="B189" t="inlineStr">
@@ -3833,16 +3833,16 @@
         </is>
       </c>
       <c r="C189" t="n">
-        <v>2016</v>
+        <v>1999</v>
       </c>
       <c r="D189" t="n">
-        <v>1840.089</v>
+        <v>289.758</v>
       </c>
     </row>
     <row r="190">
       <c r="A190" t="inlineStr">
         <is>
-          <t>New Zealand</t>
+          <t>South Korea</t>
         </is>
       </c>
       <c r="B190" t="inlineStr">
@@ -3851,16 +3851,16 @@
         </is>
       </c>
       <c r="C190" t="n">
-        <v>2015</v>
+        <v>1998</v>
       </c>
       <c r="D190" t="n">
-        <v>1782.923</v>
+        <v>239.178</v>
       </c>
     </row>
     <row r="191">
       <c r="A191" t="inlineStr">
         <is>
-          <t>New Zealand</t>
+          <t>South Korea</t>
         </is>
       </c>
       <c r="B191" t="inlineStr">
@@ -3869,16 +3869,16 @@
         </is>
       </c>
       <c r="C191" t="n">
-        <v>2014</v>
+        <v>1997</v>
       </c>
       <c r="D191" t="n">
-        <v>2049.056</v>
+        <v>333.091</v>
       </c>
     </row>
     <row r="192">
       <c r="A192" t="inlineStr">
         <is>
-          <t>New Zealand</t>
+          <t>South Korea</t>
         </is>
       </c>
       <c r="B192" t="inlineStr">
@@ -3887,16 +3887,16 @@
         </is>
       </c>
       <c r="C192" t="n">
-        <v>2013</v>
+        <v>1996</v>
       </c>
       <c r="D192" t="n">
-        <v>1954.5</v>
+        <v>358.192</v>
       </c>
     </row>
     <row r="193">
       <c r="A193" t="inlineStr">
         <is>
-          <t>New Zealand</t>
+          <t>South Korea</t>
         </is>
       </c>
       <c r="B193" t="inlineStr">
@@ -3905,16 +3905,16 @@
         </is>
       </c>
       <c r="C193" t="n">
-        <v>2012</v>
+        <v>1995</v>
       </c>
       <c r="D193" t="n">
-        <v>1895.836</v>
+        <v>342.844</v>
       </c>
     </row>
     <row r="194">
       <c r="A194" t="inlineStr">
         <is>
-          <t>New Zealand</t>
+          <t>Laos</t>
         </is>
       </c>
       <c r="B194" t="inlineStr">
@@ -3923,16 +3923,16 @@
         </is>
       </c>
       <c r="C194" t="n">
-        <v>2011</v>
+        <v>2023</v>
       </c>
       <c r="D194" t="n">
-        <v>1780.15</v>
+        <v>90.452</v>
       </c>
     </row>
     <row r="195">
       <c r="A195" t="inlineStr">
         <is>
-          <t>New Zealand</t>
+          <t>Laos</t>
         </is>
       </c>
       <c r="B195" t="inlineStr">
@@ -3941,16 +3941,16 @@
         </is>
       </c>
       <c r="C195" t="n">
-        <v>2010</v>
+        <v>2022</v>
       </c>
       <c r="D195" t="n">
-        <v>1592.41</v>
+        <v>85.499</v>
       </c>
     </row>
     <row r="196">
       <c r="A196" t="inlineStr">
         <is>
-          <t>New Zealand</t>
+          <t>Laos</t>
         </is>
       </c>
       <c r="B196" t="inlineStr">
@@ -3959,16 +3959,16 @@
         </is>
       </c>
       <c r="C196" t="n">
-        <v>2009</v>
+        <v>2021</v>
       </c>
       <c r="D196" t="n">
-        <v>1353.425</v>
+        <v>113.426</v>
       </c>
     </row>
     <row r="197">
       <c r="A197" t="inlineStr">
         <is>
-          <t>New Zealand</t>
+          <t>Laos</t>
         </is>
       </c>
       <c r="B197" t="inlineStr">
@@ -3977,16 +3977,16 @@
         </is>
       </c>
       <c r="C197" t="n">
-        <v>2008</v>
+        <v>2020</v>
       </c>
       <c r="D197" t="n">
-        <v>1461.981</v>
+        <v>121.604</v>
       </c>
     </row>
     <row r="198">
       <c r="A198" t="inlineStr">
         <is>
-          <t>New Zealand</t>
+          <t>Laos</t>
         </is>
       </c>
       <c r="B198" t="inlineStr">
@@ -3995,16 +3995,16 @@
         </is>
       </c>
       <c r="C198" t="n">
-        <v>2007</v>
+        <v>2019</v>
       </c>
       <c r="D198" t="n">
-        <v>1432.01</v>
+        <v>126.737</v>
       </c>
     </row>
     <row r="199">
       <c r="A199" t="inlineStr">
         <is>
-          <t>New Zealand</t>
+          <t>Laos</t>
         </is>
       </c>
       <c r="B199" t="inlineStr">
@@ -4013,16 +4013,16 @@
         </is>
       </c>
       <c r="C199" t="n">
-        <v>2006</v>
+        <v>2018</v>
       </c>
       <c r="D199" t="n">
-        <v>1151.255</v>
+        <v>130.932</v>
       </c>
     </row>
     <row r="200">
       <c r="A200" t="inlineStr">
         <is>
-          <t>New Zealand</t>
+          <t>Laos</t>
         </is>
       </c>
       <c r="B200" t="inlineStr">
@@ -4031,16 +4031,16 @@
         </is>
       </c>
       <c r="C200" t="n">
-        <v>2005</v>
+        <v>2017</v>
       </c>
       <c r="D200" t="n">
-        <v>1158.509</v>
+        <v>109.159</v>
       </c>
     </row>
     <row r="201">
       <c r="A201" t="inlineStr">
         <is>
-          <t>New Zealand</t>
+          <t>Laos</t>
         </is>
       </c>
       <c r="B201" t="inlineStr">
@@ -4049,16 +4049,16 @@
         </is>
       </c>
       <c r="C201" t="n">
-        <v>2004</v>
+        <v>2016</v>
       </c>
       <c r="D201" t="n">
-        <v>1033.22</v>
+        <v>110.778</v>
       </c>
     </row>
     <row r="202">
       <c r="A202" t="inlineStr">
         <is>
-          <t>New Zealand</t>
+          <t>Laos</t>
         </is>
       </c>
       <c r="B202" t="inlineStr">
@@ -4067,16 +4067,16 @@
         </is>
       </c>
       <c r="C202" t="n">
-        <v>2003</v>
+        <v>2015</v>
       </c>
       <c r="D202" t="n">
-        <v>854.8869999999999</v>
+        <v>110.734</v>
       </c>
     </row>
     <row r="203">
       <c r="A203" t="inlineStr">
         <is>
-          <t>New Zealand</t>
+          <t>Laos</t>
         </is>
       </c>
       <c r="B203" t="inlineStr">
@@ -4085,16 +4085,16 @@
         </is>
       </c>
       <c r="C203" t="n">
-        <v>2002</v>
+        <v>2014</v>
       </c>
       <c r="D203" t="n">
-        <v>640.832</v>
+        <v>77.837</v>
       </c>
     </row>
     <row r="204">
       <c r="A204" t="inlineStr">
         <is>
-          <t>New Zealand</t>
+          <t>Laos</t>
         </is>
       </c>
       <c r="B204" t="inlineStr">
@@ -4103,16 +4103,16 @@
         </is>
       </c>
       <c r="C204" t="n">
-        <v>2001</v>
+        <v>2013</v>
       </c>
       <c r="D204" t="n">
-        <v>560.647</v>
+        <v>79.916</v>
       </c>
     </row>
     <row r="205">
       <c r="A205" t="inlineStr">
         <is>
-          <t>New Zealand</t>
+          <t>Laos</t>
         </is>
       </c>
       <c r="B205" t="inlineStr">
@@ -4121,16 +4121,16 @@
         </is>
       </c>
       <c r="C205" t="n">
-        <v>2000</v>
+        <v>2012</v>
       </c>
       <c r="D205" t="n">
-        <v>594.081</v>
+        <v>78.18600000000001</v>
       </c>
     </row>
     <row r="206">
       <c r="A206" t="inlineStr">
         <is>
-          <t>New Zealand</t>
+          <t>Laos</t>
         </is>
       </c>
       <c r="B206" t="inlineStr">
@@ -4139,16 +4139,16 @@
         </is>
       </c>
       <c r="C206" t="n">
-        <v>1999</v>
+        <v>2011</v>
       </c>
       <c r="D206" t="n">
-        <v>641.6130000000001</v>
+        <v>43.342</v>
       </c>
     </row>
     <row r="207">
       <c r="A207" t="inlineStr">
         <is>
-          <t>New Zealand</t>
+          <t>Laos</t>
         </is>
       </c>
       <c r="B207" t="inlineStr">
@@ -4157,16 +4157,16 @@
         </is>
       </c>
       <c r="C207" t="n">
-        <v>1998</v>
+        <v>2010</v>
       </c>
       <c r="D207" t="n">
-        <v>648.95</v>
+        <v>42.16</v>
       </c>
     </row>
     <row r="208">
       <c r="A208" t="inlineStr">
         <is>
-          <t>New Zealand</t>
+          <t>Laos</t>
         </is>
       </c>
       <c r="B208" t="inlineStr">
@@ -4175,16 +4175,16 @@
         </is>
       </c>
       <c r="C208" t="n">
-        <v>1997</v>
+        <v>2009</v>
       </c>
       <c r="D208" t="n">
-        <v>801.629</v>
+        <v>40.887</v>
       </c>
     </row>
     <row r="209">
       <c r="A209" t="inlineStr">
         <is>
-          <t>Philippines</t>
+          <t>Laos</t>
         </is>
       </c>
       <c r="B209" t="inlineStr">
@@ -4193,16 +4193,16 @@
         </is>
       </c>
       <c r="C209" t="n">
-        <v>2023</v>
+        <v>2008</v>
       </c>
       <c r="D209" t="n">
-        <v>149.235</v>
+        <v>33.18</v>
       </c>
     </row>
     <row r="210">
       <c r="A210" t="inlineStr">
         <is>
-          <t>Philippines</t>
+          <t>Laos</t>
         </is>
       </c>
       <c r="B210" t="inlineStr">
@@ -4211,16 +4211,16 @@
         </is>
       </c>
       <c r="C210" t="n">
-        <v>2022</v>
+        <v>2007</v>
       </c>
       <c r="D210" t="n">
-        <v>147.95</v>
+        <v>20.827</v>
       </c>
     </row>
     <row r="211">
       <c r="A211" t="inlineStr">
         <is>
-          <t>Philippines</t>
+          <t>Laos</t>
         </is>
       </c>
       <c r="B211" t="inlineStr">
@@ -4229,16 +4229,16 @@
         </is>
       </c>
       <c r="C211" t="n">
-        <v>2021</v>
+        <v>2006</v>
       </c>
       <c r="D211" t="n">
-        <v>148.859</v>
+        <v>19.697</v>
       </c>
     </row>
     <row r="212">
       <c r="A212" t="inlineStr">
         <is>
-          <t>Philippines</t>
+          <t>Laos</t>
         </is>
       </c>
       <c r="B212" t="inlineStr">
@@ -4247,16 +4247,16 @@
         </is>
       </c>
       <c r="C212" t="n">
-        <v>2020</v>
+        <v>2005</v>
       </c>
       <c r="D212" t="n">
-        <v>147.751</v>
+        <v>8.784000000000001</v>
       </c>
     </row>
     <row r="213">
       <c r="A213" t="inlineStr">
         <is>
-          <t>Philippines</t>
+          <t>Laos</t>
         </is>
       </c>
       <c r="B213" t="inlineStr">
@@ -4265,16 +4265,16 @@
         </is>
       </c>
       <c r="C213" t="n">
-        <v>2019</v>
+        <v>2004</v>
       </c>
       <c r="D213" t="n">
-        <v>140.552</v>
+        <v>8.842000000000001</v>
       </c>
     </row>
     <row r="214">
       <c r="A214" t="inlineStr">
         <is>
-          <t>Philippines</t>
+          <t>Laos</t>
         </is>
       </c>
       <c r="B214" t="inlineStr">
@@ -4283,16 +4283,16 @@
         </is>
       </c>
       <c r="C214" t="n">
-        <v>2018</v>
+        <v>2003</v>
       </c>
       <c r="D214" t="n">
-        <v>138.242</v>
+        <v>8.856</v>
       </c>
     </row>
     <row r="215">
       <c r="A215" t="inlineStr">
         <is>
-          <t>Philippines</t>
+          <t>Laos</t>
         </is>
       </c>
       <c r="B215" t="inlineStr">
@@ -4301,16 +4301,16 @@
         </is>
       </c>
       <c r="C215" t="n">
-        <v>2017</v>
+        <v>2002</v>
       </c>
       <c r="D215" t="n">
-        <v>136.696</v>
+        <v>9.308</v>
       </c>
     </row>
     <row r="216">
       <c r="A216" t="inlineStr">
         <is>
-          <t>Philippines</t>
+          <t>Laos</t>
         </is>
       </c>
       <c r="B216" t="inlineStr">
@@ -4319,16 +4319,16 @@
         </is>
       </c>
       <c r="C216" t="n">
-        <v>2016</v>
+        <v>2001</v>
       </c>
       <c r="D216" t="n">
-        <v>142.338</v>
+        <v>10.453</v>
       </c>
     </row>
     <row r="217">
       <c r="A217" t="inlineStr">
         <is>
-          <t>Philippines</t>
+          <t>Laos</t>
         </is>
       </c>
       <c r="B217" t="inlineStr">
@@ -4337,16 +4337,16 @@
         </is>
       </c>
       <c r="C217" t="n">
-        <v>2015</v>
+        <v>2000</v>
       </c>
       <c r="D217" t="n">
-        <v>142.848</v>
+        <v>11.867</v>
       </c>
     </row>
     <row r="218">
       <c r="A218" t="inlineStr">
         <is>
-          <t>Philippines</t>
+          <t>Myanmar</t>
         </is>
       </c>
       <c r="B218" t="inlineStr">
@@ -4355,16 +4355,16 @@
         </is>
       </c>
       <c r="C218" t="n">
-        <v>2014</v>
+        <v>2020</v>
       </c>
       <c r="D218" t="n">
-        <v>146.412</v>
+        <v>90.32899999999999</v>
       </c>
     </row>
     <row r="219">
       <c r="A219" t="inlineStr">
         <is>
-          <t>Philippines</t>
+          <t>Myanmar</t>
         </is>
       </c>
       <c r="B219" t="inlineStr">
@@ -4373,16 +4373,16 @@
         </is>
       </c>
       <c r="C219" t="n">
-        <v>2013</v>
+        <v>2019</v>
       </c>
       <c r="D219" t="n">
-        <v>142.109</v>
+        <v>82.2</v>
       </c>
     </row>
     <row r="220">
       <c r="A220" t="inlineStr">
         <is>
-          <t>Philippines</t>
+          <t>Myanmar</t>
         </is>
       </c>
       <c r="B220" t="inlineStr">
@@ -4391,16 +4391,16 @@
         </is>
       </c>
       <c r="C220" t="n">
-        <v>2012</v>
+        <v>2018</v>
       </c>
       <c r="D220" t="n">
-        <v>142.841</v>
+        <v>87.28400000000001</v>
       </c>
     </row>
     <row r="221">
       <c r="A221" t="inlineStr">
         <is>
-          <t>Philippines</t>
+          <t>Myanmar</t>
         </is>
       </c>
       <c r="B221" t="inlineStr">
@@ -4409,16 +4409,16 @@
         </is>
       </c>
       <c r="C221" t="n">
-        <v>2011</v>
+        <v>2017</v>
       </c>
       <c r="D221" t="n">
-        <v>139.265</v>
+        <v>68.80500000000001</v>
       </c>
     </row>
     <row r="222">
       <c r="A222" t="inlineStr">
         <is>
-          <t>Philippines</t>
+          <t>Myanmar</t>
         </is>
       </c>
       <c r="B222" t="inlineStr">
@@ -4427,16 +4427,16 @@
         </is>
       </c>
       <c r="C222" t="n">
-        <v>2010</v>
+        <v>2016</v>
       </c>
       <c r="D222" t="n">
-        <v>127.955</v>
+        <v>75.798</v>
       </c>
     </row>
     <row r="223">
       <c r="A223" t="inlineStr">
         <is>
-          <t>Philippines</t>
+          <t>Myanmar</t>
         </is>
       </c>
       <c r="B223" t="inlineStr">
@@ -4445,16 +4445,16 @@
         </is>
       </c>
       <c r="C223" t="n">
-        <v>2009</v>
+        <v>2015</v>
       </c>
       <c r="D223" t="n">
-        <v>208.978</v>
+        <v>80.508</v>
       </c>
     </row>
     <row r="224">
       <c r="A224" t="inlineStr">
         <is>
-          <t>Philippines</t>
+          <t>Malaysia</t>
         </is>
       </c>
       <c r="B224" t="inlineStr">
@@ -4463,16 +4463,16 @@
         </is>
       </c>
       <c r="C224" t="n">
-        <v>2008</v>
+        <v>2023</v>
       </c>
       <c r="D224" t="n">
-        <v>224.803</v>
+        <v>328.902</v>
       </c>
     </row>
     <row r="225">
       <c r="A225" t="inlineStr">
         <is>
-          <t>Philippines</t>
+          <t>Malaysia</t>
         </is>
       </c>
       <c r="B225" t="inlineStr">
@@ -4481,16 +4481,16 @@
         </is>
       </c>
       <c r="C225" t="n">
-        <v>2007</v>
+        <v>2022</v>
       </c>
       <c r="D225" t="n">
-        <v>204.601</v>
+        <v>340.826</v>
       </c>
     </row>
     <row r="226">
       <c r="A226" t="inlineStr">
         <is>
-          <t>Philippines</t>
+          <t>Malaysia</t>
         </is>
       </c>
       <c r="B226" t="inlineStr">
@@ -4499,16 +4499,16 @@
         </is>
       </c>
       <c r="C226" t="n">
-        <v>2006</v>
+        <v>2021</v>
       </c>
       <c r="D226" t="n">
-        <v>177.904</v>
+        <v>289.624</v>
       </c>
     </row>
     <row r="227">
       <c r="A227" t="inlineStr">
         <is>
-          <t>Philippines</t>
+          <t>Malaysia</t>
         </is>
       </c>
       <c r="B227" t="inlineStr">
@@ -4517,16 +4517,16 @@
         </is>
       </c>
       <c r="C227" t="n">
-        <v>2005</v>
+        <v>2020</v>
       </c>
       <c r="D227" t="n">
-        <v>153.888</v>
+        <v>285.478</v>
       </c>
     </row>
     <row r="228">
       <c r="A228" t="inlineStr">
         <is>
-          <t>Philippines</t>
+          <t>Malaysia</t>
         </is>
       </c>
       <c r="B228" t="inlineStr">
@@ -4535,16 +4535,16 @@
         </is>
       </c>
       <c r="C228" t="n">
-        <v>2004</v>
+        <v>2019</v>
       </c>
       <c r="D228" t="n">
-        <v>139.633</v>
+        <v>265.542</v>
       </c>
     </row>
     <row r="229">
       <c r="A229" t="inlineStr">
         <is>
-          <t>Philippines</t>
+          <t>Malaysia</t>
         </is>
       </c>
       <c r="B229" t="inlineStr">
@@ -4553,16 +4553,16 @@
         </is>
       </c>
       <c r="C229" t="n">
-        <v>2003</v>
+        <v>2018</v>
       </c>
       <c r="D229" t="n">
-        <v>134.733</v>
+        <v>247.823</v>
       </c>
     </row>
     <row r="230">
       <c r="A230" t="inlineStr">
         <is>
-          <t>Philippines</t>
+          <t>Malaysia</t>
         </is>
       </c>
       <c r="B230" t="inlineStr">
@@ -4571,16 +4571,16 @@
         </is>
       </c>
       <c r="C230" t="n">
-        <v>2002</v>
+        <v>2017</v>
       </c>
       <c r="D230" t="n">
-        <v>141.521</v>
+        <v>232.534</v>
       </c>
     </row>
     <row r="231">
       <c r="A231" t="inlineStr">
         <is>
-          <t>Philippines</t>
+          <t>Malaysia</t>
         </is>
       </c>
       <c r="B231" t="inlineStr">
@@ -4589,16 +4589,16 @@
         </is>
       </c>
       <c r="C231" t="n">
-        <v>2001</v>
+        <v>2016</v>
       </c>
       <c r="D231" t="n">
-        <v>135.549</v>
+        <v>241.063</v>
       </c>
     </row>
     <row r="232">
       <c r="A232" t="inlineStr">
         <is>
-          <t>Philippines</t>
+          <t>Malaysia</t>
         </is>
       </c>
       <c r="B232" t="inlineStr">
@@ -4607,16 +4607,16 @@
         </is>
       </c>
       <c r="C232" t="n">
-        <v>2000</v>
+        <v>2015</v>
       </c>
       <c r="D232" t="n">
-        <v>147.56</v>
+        <v>230.444</v>
       </c>
     </row>
     <row r="233">
       <c r="A233" t="inlineStr">
         <is>
-          <t>Philippines</t>
+          <t>Malaysia</t>
         </is>
       </c>
       <c r="B233" t="inlineStr">
@@ -4625,16 +4625,16 @@
         </is>
       </c>
       <c r="C233" t="n">
-        <v>1999</v>
+        <v>2014</v>
       </c>
       <c r="D233" t="n">
-        <v>149.147</v>
+        <v>274.989</v>
       </c>
     </row>
     <row r="234">
       <c r="A234" t="inlineStr">
         <is>
-          <t>Philippines</t>
+          <t>Malaysia</t>
         </is>
       </c>
       <c r="B234" t="inlineStr">
@@ -4643,16 +4643,16 @@
         </is>
       </c>
       <c r="C234" t="n">
-        <v>1998</v>
+        <v>2013</v>
       </c>
       <c r="D234" t="n">
-        <v>126.305</v>
+        <v>285.632</v>
       </c>
     </row>
     <row r="235">
       <c r="A235" t="inlineStr">
         <is>
-          <t>Philippines</t>
+          <t>New Zealand</t>
         </is>
       </c>
       <c r="B235" t="inlineStr">
@@ -4661,16 +4661,16 @@
         </is>
       </c>
       <c r="C235" t="n">
-        <v>1997</v>
+        <v>2023</v>
       </c>
       <c r="D235" t="n">
-        <v>163.722</v>
+        <v>2414.37</v>
       </c>
     </row>
     <row r="236">
       <c r="A236" t="inlineStr">
         <is>
-          <t>Philippines</t>
+          <t>New Zealand</t>
         </is>
       </c>
       <c r="B236" t="inlineStr">
@@ -4679,16 +4679,16 @@
         </is>
       </c>
       <c r="C236" t="n">
-        <v>1996</v>
+        <v>2022</v>
       </c>
       <c r="D236" t="n">
-        <v>164.174</v>
+        <v>2329.892</v>
       </c>
     </row>
     <row r="237">
       <c r="A237" t="inlineStr">
         <is>
-          <t>Philippines</t>
+          <t>New Zealand</t>
         </is>
       </c>
       <c r="B237" t="inlineStr">
@@ -4697,16 +4697,16 @@
         </is>
       </c>
       <c r="C237" t="n">
-        <v>1995</v>
+        <v>2021</v>
       </c>
       <c r="D237" t="n">
-        <v>147.077</v>
+        <v>2452.021</v>
       </c>
     </row>
     <row r="238">
       <c r="A238" t="inlineStr">
         <is>
-          <t>Thailand</t>
+          <t>New Zealand</t>
         </is>
       </c>
       <c r="B238" t="inlineStr">
@@ -4715,16 +4715,16 @@
         </is>
       </c>
       <c r="C238" t="n">
-        <v>2023</v>
+        <v>2020</v>
       </c>
       <c r="D238" t="n">
-        <v>250.272</v>
+        <v>2124.433</v>
       </c>
     </row>
     <row r="239">
       <c r="A239" t="inlineStr">
         <is>
-          <t>Thailand</t>
+          <t>New Zealand</t>
         </is>
       </c>
       <c r="B239" t="inlineStr">
@@ -4733,16 +4733,16 @@
         </is>
       </c>
       <c r="C239" t="n">
-        <v>2022</v>
+        <v>2019</v>
       </c>
       <c r="D239" t="n">
-        <v>248.422</v>
+        <v>2021.247</v>
       </c>
     </row>
     <row r="240">
       <c r="A240" t="inlineStr">
         <is>
-          <t>Thailand</t>
+          <t>New Zealand</t>
         </is>
       </c>
       <c r="B240" t="inlineStr">
@@ -4751,16 +4751,16 @@
         </is>
       </c>
       <c r="C240" t="n">
-        <v>2021</v>
+        <v>2018</v>
       </c>
       <c r="D240" t="n">
-        <v>260.186</v>
+        <v>1978.885</v>
       </c>
     </row>
     <row r="241">
       <c r="A241" t="inlineStr">
         <is>
-          <t>Thailand</t>
+          <t>New Zealand</t>
         </is>
       </c>
       <c r="B241" t="inlineStr">
@@ -4769,16 +4769,16 @@
         </is>
       </c>
       <c r="C241" t="n">
-        <v>2020</v>
+        <v>2017</v>
       </c>
       <c r="D241" t="n">
-        <v>265.868</v>
+        <v>1939.736</v>
       </c>
     </row>
     <row r="242">
       <c r="A242" t="inlineStr">
         <is>
-          <t>Thailand</t>
+          <t>New Zealand</t>
         </is>
       </c>
       <c r="B242" t="inlineStr">
@@ -4787,16 +4787,16 @@
         </is>
       </c>
       <c r="C242" t="n">
-        <v>2019</v>
+        <v>2016</v>
       </c>
       <c r="D242" t="n">
-        <v>263.788</v>
+        <v>1840.089</v>
       </c>
     </row>
     <row r="243">
       <c r="A243" t="inlineStr">
         <is>
-          <t>Thailand</t>
+          <t>New Zealand</t>
         </is>
       </c>
       <c r="B243" t="inlineStr">
@@ -4805,16 +4805,16 @@
         </is>
       </c>
       <c r="C243" t="n">
-        <v>2018</v>
+        <v>2015</v>
       </c>
       <c r="D243" t="n">
-        <v>253.48</v>
+        <v>1782.923</v>
       </c>
     </row>
     <row r="244">
       <c r="A244" t="inlineStr">
         <is>
-          <t>Thailand</t>
+          <t>New Zealand</t>
         </is>
       </c>
       <c r="B244" t="inlineStr">
@@ -4823,16 +4823,16 @@
         </is>
       </c>
       <c r="C244" t="n">
-        <v>2017</v>
+        <v>2014</v>
       </c>
       <c r="D244" t="n">
-        <v>233.649</v>
+        <v>2049.056</v>
       </c>
     </row>
     <row r="245">
       <c r="A245" t="inlineStr">
         <is>
-          <t>Thailand</t>
+          <t>New Zealand</t>
         </is>
       </c>
       <c r="B245" t="inlineStr">
@@ -4841,16 +4841,16 @@
         </is>
       </c>
       <c r="C245" t="n">
-        <v>2016</v>
+        <v>2013</v>
       </c>
       <c r="D245" t="n">
-        <v>220.986</v>
+        <v>1954.5</v>
       </c>
     </row>
     <row r="246">
       <c r="A246" t="inlineStr">
         <is>
-          <t>Thailand</t>
+          <t>New Zealand</t>
         </is>
       </c>
       <c r="B246" t="inlineStr">
@@ -4859,16 +4859,16 @@
         </is>
       </c>
       <c r="C246" t="n">
-        <v>2015</v>
+        <v>2012</v>
       </c>
       <c r="D246" t="n">
-        <v>227.752</v>
+        <v>1895.836</v>
       </c>
     </row>
     <row r="247">
       <c r="A247" t="inlineStr">
         <is>
-          <t>Thailand</t>
+          <t>New Zealand</t>
         </is>
       </c>
       <c r="B247" t="inlineStr">
@@ -4877,16 +4877,16 @@
         </is>
       </c>
       <c r="C247" t="n">
-        <v>2014</v>
+        <v>2011</v>
       </c>
       <c r="D247" t="n">
-        <v>240.149</v>
+        <v>1780.15</v>
       </c>
     </row>
     <row r="248">
       <c r="A248" t="inlineStr">
         <is>
-          <t>Thailand</t>
+          <t>New Zealand</t>
         </is>
       </c>
       <c r="B248" t="inlineStr">
@@ -4895,16 +4895,16 @@
         </is>
       </c>
       <c r="C248" t="n">
-        <v>2013</v>
+        <v>2010</v>
       </c>
       <c r="D248" t="n">
-        <v>253.857</v>
+        <v>1592.41</v>
       </c>
     </row>
     <row r="249">
       <c r="A249" t="inlineStr">
         <is>
-          <t>Thailand</t>
+          <t>New Zealand</t>
         </is>
       </c>
       <c r="B249" t="inlineStr">
@@ -4913,16 +4913,16 @@
         </is>
       </c>
       <c r="C249" t="n">
-        <v>2012</v>
+        <v>2009</v>
       </c>
       <c r="D249" t="n">
-        <v>199.916</v>
+        <v>1353.425</v>
       </c>
     </row>
     <row r="250">
       <c r="A250" t="inlineStr">
         <is>
-          <t>Thailand</t>
+          <t>New Zealand</t>
         </is>
       </c>
       <c r="B250" t="inlineStr">
@@ -4931,16 +4931,16 @@
         </is>
       </c>
       <c r="C250" t="n">
-        <v>2011</v>
+        <v>2008</v>
       </c>
       <c r="D250" t="n">
-        <v>145.81</v>
+        <v>1461.981</v>
       </c>
     </row>
     <row r="251">
       <c r="A251" t="inlineStr">
         <is>
-          <t>Thailand</t>
+          <t>New Zealand</t>
         </is>
       </c>
       <c r="B251" t="inlineStr">
@@ -4949,16 +4949,16 @@
         </is>
       </c>
       <c r="C251" t="n">
-        <v>2010</v>
+        <v>2007</v>
       </c>
       <c r="D251" t="n">
-        <v>131.29</v>
+        <v>1432.01</v>
       </c>
     </row>
     <row r="252">
       <c r="A252" t="inlineStr">
         <is>
-          <t>Thailand</t>
+          <t>New Zealand</t>
         </is>
       </c>
       <c r="B252" t="inlineStr">
@@ -4967,16 +4967,16 @@
         </is>
       </c>
       <c r="C252" t="n">
-        <v>2009</v>
+        <v>2006</v>
       </c>
       <c r="D252" t="n">
-        <v>117.542</v>
+        <v>1151.255</v>
       </c>
     </row>
     <row r="253">
       <c r="A253" t="inlineStr">
         <is>
-          <t>Thailand</t>
+          <t>New Zealand</t>
         </is>
       </c>
       <c r="B253" t="inlineStr">
@@ -4985,16 +4985,16 @@
         </is>
       </c>
       <c r="C253" t="n">
-        <v>2008</v>
+        <v>2005</v>
       </c>
       <c r="D253" t="n">
-        <v>120.973</v>
+        <v>1158.509</v>
       </c>
     </row>
     <row r="254">
       <c r="A254" t="inlineStr">
         <is>
-          <t>Thailand</t>
+          <t>New Zealand</t>
         </is>
       </c>
       <c r="B254" t="inlineStr">
@@ -5003,16 +5003,16 @@
         </is>
       </c>
       <c r="C254" t="n">
-        <v>2007</v>
+        <v>2004</v>
       </c>
       <c r="D254" t="n">
-        <v>143.866</v>
+        <v>1033.22</v>
       </c>
     </row>
     <row r="255">
       <c r="A255" t="inlineStr">
         <is>
-          <t>Thailand</t>
+          <t>New Zealand</t>
         </is>
       </c>
       <c r="B255" t="inlineStr">
@@ -5021,16 +5021,16 @@
         </is>
       </c>
       <c r="C255" t="n">
-        <v>2006</v>
+        <v>2003</v>
       </c>
       <c r="D255" t="n">
-        <v>126.287</v>
+        <v>854.8869999999999</v>
       </c>
     </row>
     <row r="256">
       <c r="A256" t="inlineStr">
         <is>
-          <t>Thailand</t>
+          <t>New Zealand</t>
         </is>
       </c>
       <c r="B256" t="inlineStr">
@@ -5039,16 +5039,16 @@
         </is>
       </c>
       <c r="C256" t="n">
-        <v>2005</v>
+        <v>2002</v>
       </c>
       <c r="D256" t="n">
-        <v>115.067</v>
+        <v>640.832</v>
       </c>
     </row>
     <row r="257">
       <c r="A257" t="inlineStr">
         <is>
-          <t>Thailand</t>
+          <t>New Zealand</t>
         </is>
       </c>
       <c r="B257" t="inlineStr">
@@ -5057,16 +5057,16 @@
         </is>
       </c>
       <c r="C257" t="n">
-        <v>2004</v>
+        <v>2001</v>
       </c>
       <c r="D257" t="n">
-        <v>109.889</v>
+        <v>560.647</v>
       </c>
     </row>
     <row r="258">
       <c r="A258" t="inlineStr">
         <is>
-          <t>Thailand</t>
+          <t>New Zealand</t>
         </is>
       </c>
       <c r="B258" t="inlineStr">
@@ -5075,16 +5075,16 @@
         </is>
       </c>
       <c r="C258" t="n">
-        <v>2003</v>
+        <v>2000</v>
       </c>
       <c r="D258" t="n">
-        <v>105.919</v>
+        <v>594.081</v>
       </c>
     </row>
     <row r="259">
       <c r="A259" t="inlineStr">
         <is>
-          <t>Thailand</t>
+          <t>New Zealand</t>
         </is>
       </c>
       <c r="B259" t="inlineStr">
@@ -5093,16 +5093,16 @@
         </is>
       </c>
       <c r="C259" t="n">
-        <v>2002</v>
+        <v>1999</v>
       </c>
       <c r="D259" t="n">
-        <v>99.86</v>
+        <v>641.6130000000001</v>
       </c>
     </row>
     <row r="260">
       <c r="A260" t="inlineStr">
         <is>
-          <t>Thailand</t>
+          <t>New Zealand</t>
         </is>
       </c>
       <c r="B260" t="inlineStr">
@@ -5111,16 +5111,16 @@
         </is>
       </c>
       <c r="C260" t="n">
-        <v>2001</v>
+        <v>1998</v>
       </c>
       <c r="D260" t="n">
-        <v>96.55200000000001</v>
+        <v>648.95</v>
       </c>
     </row>
     <row r="261">
       <c r="A261" t="inlineStr">
         <is>
-          <t>Thailand</t>
+          <t>New Zealand</t>
         </is>
       </c>
       <c r="B261" t="inlineStr">
@@ -5129,16 +5129,16 @@
         </is>
       </c>
       <c r="C261" t="n">
-        <v>2000</v>
+        <v>1997</v>
       </c>
       <c r="D261" t="n">
-        <v>105.006</v>
+        <v>801.629</v>
       </c>
     </row>
     <row r="262">
       <c r="A262" t="inlineStr">
         <is>
-          <t>Thailand</t>
+          <t>Philippines</t>
         </is>
       </c>
       <c r="B262" t="inlineStr">
@@ -5147,16 +5147,16 @@
         </is>
       </c>
       <c r="C262" t="n">
-        <v>1999</v>
+        <v>2023</v>
       </c>
       <c r="D262" t="n">
-        <v>111.388</v>
+        <v>149.235</v>
       </c>
     </row>
     <row r="263">
       <c r="A263" t="inlineStr">
         <is>
-          <t>Thailand</t>
+          <t>Philippines</t>
         </is>
       </c>
       <c r="B263" t="inlineStr">
@@ -5165,16 +5165,16 @@
         </is>
       </c>
       <c r="C263" t="n">
-        <v>1998</v>
+        <v>2022</v>
       </c>
       <c r="D263" t="n">
-        <v>101.839</v>
+        <v>147.95</v>
       </c>
     </row>
     <row r="264">
       <c r="A264" t="inlineStr">
         <is>
-          <t>Thailand</t>
+          <t>Philippines</t>
         </is>
       </c>
       <c r="B264" t="inlineStr">
@@ -5183,16 +5183,16 @@
         </is>
       </c>
       <c r="C264" t="n">
-        <v>1997</v>
+        <v>2021</v>
       </c>
       <c r="D264" t="n">
-        <v>130.148</v>
+        <v>148.859</v>
       </c>
     </row>
     <row r="265">
       <c r="A265" t="inlineStr">
         <is>
-          <t>Thailand</t>
+          <t>Philippines</t>
         </is>
       </c>
       <c r="B265" t="inlineStr">
@@ -5201,28 +5201,1414 @@
         </is>
       </c>
       <c r="C265" t="n">
-        <v>1996</v>
+        <v>2020</v>
       </c>
       <c r="D265" t="n">
-        <v>161.072</v>
+        <v>147.751</v>
       </c>
     </row>
     <row r="266">
       <c r="A266" t="inlineStr">
         <is>
+          <t>Philippines</t>
+        </is>
+      </c>
+      <c r="B266" t="inlineStr">
+        <is>
+          <t>Currency: U.S. dollars</t>
+        </is>
+      </c>
+      <c r="C266" t="n">
+        <v>2019</v>
+      </c>
+      <c r="D266" t="n">
+        <v>140.552</v>
+      </c>
+    </row>
+    <row r="267">
+      <c r="A267" t="inlineStr">
+        <is>
+          <t>Philippines</t>
+        </is>
+      </c>
+      <c r="B267" t="inlineStr">
+        <is>
+          <t>Currency: U.S. dollars</t>
+        </is>
+      </c>
+      <c r="C267" t="n">
+        <v>2018</v>
+      </c>
+      <c r="D267" t="n">
+        <v>138.242</v>
+      </c>
+    </row>
+    <row r="268">
+      <c r="A268" t="inlineStr">
+        <is>
+          <t>Philippines</t>
+        </is>
+      </c>
+      <c r="B268" t="inlineStr">
+        <is>
+          <t>Currency: U.S. dollars</t>
+        </is>
+      </c>
+      <c r="C268" t="n">
+        <v>2017</v>
+      </c>
+      <c r="D268" t="n">
+        <v>136.696</v>
+      </c>
+    </row>
+    <row r="269">
+      <c r="A269" t="inlineStr">
+        <is>
+          <t>Philippines</t>
+        </is>
+      </c>
+      <c r="B269" t="inlineStr">
+        <is>
+          <t>Currency: U.S. dollars</t>
+        </is>
+      </c>
+      <c r="C269" t="n">
+        <v>2016</v>
+      </c>
+      <c r="D269" t="n">
+        <v>142.338</v>
+      </c>
+    </row>
+    <row r="270">
+      <c r="A270" t="inlineStr">
+        <is>
+          <t>Philippines</t>
+        </is>
+      </c>
+      <c r="B270" t="inlineStr">
+        <is>
+          <t>Currency: U.S. dollars</t>
+        </is>
+      </c>
+      <c r="C270" t="n">
+        <v>2015</v>
+      </c>
+      <c r="D270" t="n">
+        <v>142.848</v>
+      </c>
+    </row>
+    <row r="271">
+      <c r="A271" t="inlineStr">
+        <is>
+          <t>Philippines</t>
+        </is>
+      </c>
+      <c r="B271" t="inlineStr">
+        <is>
+          <t>Currency: U.S. dollars</t>
+        </is>
+      </c>
+      <c r="C271" t="n">
+        <v>2014</v>
+      </c>
+      <c r="D271" t="n">
+        <v>146.412</v>
+      </c>
+    </row>
+    <row r="272">
+      <c r="A272" t="inlineStr">
+        <is>
+          <t>Philippines</t>
+        </is>
+      </c>
+      <c r="B272" t="inlineStr">
+        <is>
+          <t>Currency: U.S. dollars</t>
+        </is>
+      </c>
+      <c r="C272" t="n">
+        <v>2013</v>
+      </c>
+      <c r="D272" t="n">
+        <v>142.109</v>
+      </c>
+    </row>
+    <row r="273">
+      <c r="A273" t="inlineStr">
+        <is>
+          <t>Philippines</t>
+        </is>
+      </c>
+      <c r="B273" t="inlineStr">
+        <is>
+          <t>Currency: U.S. dollars</t>
+        </is>
+      </c>
+      <c r="C273" t="n">
+        <v>2012</v>
+      </c>
+      <c r="D273" t="n">
+        <v>142.841</v>
+      </c>
+    </row>
+    <row r="274">
+      <c r="A274" t="inlineStr">
+        <is>
+          <t>Philippines</t>
+        </is>
+      </c>
+      <c r="B274" t="inlineStr">
+        <is>
+          <t>Currency: U.S. dollars</t>
+        </is>
+      </c>
+      <c r="C274" t="n">
+        <v>2011</v>
+      </c>
+      <c r="D274" t="n">
+        <v>139.265</v>
+      </c>
+    </row>
+    <row r="275">
+      <c r="A275" t="inlineStr">
+        <is>
+          <t>Philippines</t>
+        </is>
+      </c>
+      <c r="B275" t="inlineStr">
+        <is>
+          <t>Currency: U.S. dollars</t>
+        </is>
+      </c>
+      <c r="C275" t="n">
+        <v>2010</v>
+      </c>
+      <c r="D275" t="n">
+        <v>127.955</v>
+      </c>
+    </row>
+    <row r="276">
+      <c r="A276" t="inlineStr">
+        <is>
+          <t>Philippines</t>
+        </is>
+      </c>
+      <c r="B276" t="inlineStr">
+        <is>
+          <t>Currency: U.S. dollars</t>
+        </is>
+      </c>
+      <c r="C276" t="n">
+        <v>2009</v>
+      </c>
+      <c r="D276" t="n">
+        <v>208.978</v>
+      </c>
+    </row>
+    <row r="277">
+      <c r="A277" t="inlineStr">
+        <is>
+          <t>Philippines</t>
+        </is>
+      </c>
+      <c r="B277" t="inlineStr">
+        <is>
+          <t>Currency: U.S. dollars</t>
+        </is>
+      </c>
+      <c r="C277" t="n">
+        <v>2008</v>
+      </c>
+      <c r="D277" t="n">
+        <v>224.803</v>
+      </c>
+    </row>
+    <row r="278">
+      <c r="A278" t="inlineStr">
+        <is>
+          <t>Philippines</t>
+        </is>
+      </c>
+      <c r="B278" t="inlineStr">
+        <is>
+          <t>Currency: U.S. dollars</t>
+        </is>
+      </c>
+      <c r="C278" t="n">
+        <v>2007</v>
+      </c>
+      <c r="D278" t="n">
+        <v>204.601</v>
+      </c>
+    </row>
+    <row r="279">
+      <c r="A279" t="inlineStr">
+        <is>
+          <t>Philippines</t>
+        </is>
+      </c>
+      <c r="B279" t="inlineStr">
+        <is>
+          <t>Currency: U.S. dollars</t>
+        </is>
+      </c>
+      <c r="C279" t="n">
+        <v>2006</v>
+      </c>
+      <c r="D279" t="n">
+        <v>177.904</v>
+      </c>
+    </row>
+    <row r="280">
+      <c r="A280" t="inlineStr">
+        <is>
+          <t>Philippines</t>
+        </is>
+      </c>
+      <c r="B280" t="inlineStr">
+        <is>
+          <t>Currency: U.S. dollars</t>
+        </is>
+      </c>
+      <c r="C280" t="n">
+        <v>2005</v>
+      </c>
+      <c r="D280" t="n">
+        <v>153.888</v>
+      </c>
+    </row>
+    <row r="281">
+      <c r="A281" t="inlineStr">
+        <is>
+          <t>Philippines</t>
+        </is>
+      </c>
+      <c r="B281" t="inlineStr">
+        <is>
+          <t>Currency: U.S. dollars</t>
+        </is>
+      </c>
+      <c r="C281" t="n">
+        <v>2004</v>
+      </c>
+      <c r="D281" t="n">
+        <v>139.633</v>
+      </c>
+    </row>
+    <row r="282">
+      <c r="A282" t="inlineStr">
+        <is>
+          <t>Philippines</t>
+        </is>
+      </c>
+      <c r="B282" t="inlineStr">
+        <is>
+          <t>Currency: U.S. dollars</t>
+        </is>
+      </c>
+      <c r="C282" t="n">
+        <v>2003</v>
+      </c>
+      <c r="D282" t="n">
+        <v>134.733</v>
+      </c>
+    </row>
+    <row r="283">
+      <c r="A283" t="inlineStr">
+        <is>
+          <t>Philippines</t>
+        </is>
+      </c>
+      <c r="B283" t="inlineStr">
+        <is>
+          <t>Currency: U.S. dollars</t>
+        </is>
+      </c>
+      <c r="C283" t="n">
+        <v>2002</v>
+      </c>
+      <c r="D283" t="n">
+        <v>141.521</v>
+      </c>
+    </row>
+    <row r="284">
+      <c r="A284" t="inlineStr">
+        <is>
+          <t>Philippines</t>
+        </is>
+      </c>
+      <c r="B284" t="inlineStr">
+        <is>
+          <t>Currency: U.S. dollars</t>
+        </is>
+      </c>
+      <c r="C284" t="n">
+        <v>2001</v>
+      </c>
+      <c r="D284" t="n">
+        <v>135.549</v>
+      </c>
+    </row>
+    <row r="285">
+      <c r="A285" t="inlineStr">
+        <is>
+          <t>Philippines</t>
+        </is>
+      </c>
+      <c r="B285" t="inlineStr">
+        <is>
+          <t>Currency: U.S. dollars</t>
+        </is>
+      </c>
+      <c r="C285" t="n">
+        <v>2000</v>
+      </c>
+      <c r="D285" t="n">
+        <v>147.56</v>
+      </c>
+    </row>
+    <row r="286">
+      <c r="A286" t="inlineStr">
+        <is>
+          <t>Philippines</t>
+        </is>
+      </c>
+      <c r="B286" t="inlineStr">
+        <is>
+          <t>Currency: U.S. dollars</t>
+        </is>
+      </c>
+      <c r="C286" t="n">
+        <v>1999</v>
+      </c>
+      <c r="D286" t="n">
+        <v>149.147</v>
+      </c>
+    </row>
+    <row r="287">
+      <c r="A287" t="inlineStr">
+        <is>
+          <t>Philippines</t>
+        </is>
+      </c>
+      <c r="B287" t="inlineStr">
+        <is>
+          <t>Currency: U.S. dollars</t>
+        </is>
+      </c>
+      <c r="C287" t="n">
+        <v>1998</v>
+      </c>
+      <c r="D287" t="n">
+        <v>126.305</v>
+      </c>
+    </row>
+    <row r="288">
+      <c r="A288" t="inlineStr">
+        <is>
+          <t>Philippines</t>
+        </is>
+      </c>
+      <c r="B288" t="inlineStr">
+        <is>
+          <t>Currency: U.S. dollars</t>
+        </is>
+      </c>
+      <c r="C288" t="n">
+        <v>1997</v>
+      </c>
+      <c r="D288" t="n">
+        <v>163.722</v>
+      </c>
+    </row>
+    <row r="289">
+      <c r="A289" t="inlineStr">
+        <is>
+          <t>Philippines</t>
+        </is>
+      </c>
+      <c r="B289" t="inlineStr">
+        <is>
+          <t>Currency: U.S. dollars</t>
+        </is>
+      </c>
+      <c r="C289" t="n">
+        <v>1996</v>
+      </c>
+      <c r="D289" t="n">
+        <v>164.174</v>
+      </c>
+    </row>
+    <row r="290">
+      <c r="A290" t="inlineStr">
+        <is>
+          <t>Philippines</t>
+        </is>
+      </c>
+      <c r="B290" t="inlineStr">
+        <is>
+          <t>Currency: U.S. dollars</t>
+        </is>
+      </c>
+      <c r="C290" t="n">
+        <v>1995</v>
+      </c>
+      <c r="D290" t="n">
+        <v>147.077</v>
+      </c>
+    </row>
+    <row r="291">
+      <c r="A291" t="inlineStr">
+        <is>
           <t>Thailand</t>
         </is>
       </c>
-      <c r="B266" t="inlineStr">
-        <is>
-          <t>Currency: U.S. dollars</t>
-        </is>
-      </c>
-      <c r="C266" t="n">
+      <c r="B291" t="inlineStr">
+        <is>
+          <t>Currency: U.S. dollars</t>
+        </is>
+      </c>
+      <c r="C291" t="n">
+        <v>2023</v>
+      </c>
+      <c r="D291" t="n">
+        <v>250.272</v>
+      </c>
+    </row>
+    <row r="292">
+      <c r="A292" t="inlineStr">
+        <is>
+          <t>Thailand</t>
+        </is>
+      </c>
+      <c r="B292" t="inlineStr">
+        <is>
+          <t>Currency: U.S. dollars</t>
+        </is>
+      </c>
+      <c r="C292" t="n">
+        <v>2022</v>
+      </c>
+      <c r="D292" t="n">
+        <v>248.422</v>
+      </c>
+    </row>
+    <row r="293">
+      <c r="A293" t="inlineStr">
+        <is>
+          <t>Thailand</t>
+        </is>
+      </c>
+      <c r="B293" t="inlineStr">
+        <is>
+          <t>Currency: U.S. dollars</t>
+        </is>
+      </c>
+      <c r="C293" t="n">
+        <v>2021</v>
+      </c>
+      <c r="D293" t="n">
+        <v>260.186</v>
+      </c>
+    </row>
+    <row r="294">
+      <c r="A294" t="inlineStr">
+        <is>
+          <t>Thailand</t>
+        </is>
+      </c>
+      <c r="B294" t="inlineStr">
+        <is>
+          <t>Currency: U.S. dollars</t>
+        </is>
+      </c>
+      <c r="C294" t="n">
+        <v>2020</v>
+      </c>
+      <c r="D294" t="n">
+        <v>265.868</v>
+      </c>
+    </row>
+    <row r="295">
+      <c r="A295" t="inlineStr">
+        <is>
+          <t>Thailand</t>
+        </is>
+      </c>
+      <c r="B295" t="inlineStr">
+        <is>
+          <t>Currency: U.S. dollars</t>
+        </is>
+      </c>
+      <c r="C295" t="n">
+        <v>2019</v>
+      </c>
+      <c r="D295" t="n">
+        <v>263.788</v>
+      </c>
+    </row>
+    <row r="296">
+      <c r="A296" t="inlineStr">
+        <is>
+          <t>Thailand</t>
+        </is>
+      </c>
+      <c r="B296" t="inlineStr">
+        <is>
+          <t>Currency: U.S. dollars</t>
+        </is>
+      </c>
+      <c r="C296" t="n">
+        <v>2018</v>
+      </c>
+      <c r="D296" t="n">
+        <v>253.48</v>
+      </c>
+    </row>
+    <row r="297">
+      <c r="A297" t="inlineStr">
+        <is>
+          <t>Thailand</t>
+        </is>
+      </c>
+      <c r="B297" t="inlineStr">
+        <is>
+          <t>Currency: U.S. dollars</t>
+        </is>
+      </c>
+      <c r="C297" t="n">
+        <v>2017</v>
+      </c>
+      <c r="D297" t="n">
+        <v>233.649</v>
+      </c>
+    </row>
+    <row r="298">
+      <c r="A298" t="inlineStr">
+        <is>
+          <t>Thailand</t>
+        </is>
+      </c>
+      <c r="B298" t="inlineStr">
+        <is>
+          <t>Currency: U.S. dollars</t>
+        </is>
+      </c>
+      <c r="C298" t="n">
+        <v>2016</v>
+      </c>
+      <c r="D298" t="n">
+        <v>220.986</v>
+      </c>
+    </row>
+    <row r="299">
+      <c r="A299" t="inlineStr">
+        <is>
+          <t>Thailand</t>
+        </is>
+      </c>
+      <c r="B299" t="inlineStr">
+        <is>
+          <t>Currency: U.S. dollars</t>
+        </is>
+      </c>
+      <c r="C299" t="n">
+        <v>2015</v>
+      </c>
+      <c r="D299" t="n">
+        <v>227.752</v>
+      </c>
+    </row>
+    <row r="300">
+      <c r="A300" t="inlineStr">
+        <is>
+          <t>Thailand</t>
+        </is>
+      </c>
+      <c r="B300" t="inlineStr">
+        <is>
+          <t>Currency: U.S. dollars</t>
+        </is>
+      </c>
+      <c r="C300" t="n">
+        <v>2014</v>
+      </c>
+      <c r="D300" t="n">
+        <v>240.149</v>
+      </c>
+    </row>
+    <row r="301">
+      <c r="A301" t="inlineStr">
+        <is>
+          <t>Thailand</t>
+        </is>
+      </c>
+      <c r="B301" t="inlineStr">
+        <is>
+          <t>Currency: U.S. dollars</t>
+        </is>
+      </c>
+      <c r="C301" t="n">
+        <v>2013</v>
+      </c>
+      <c r="D301" t="n">
+        <v>253.857</v>
+      </c>
+    </row>
+    <row r="302">
+      <c r="A302" t="inlineStr">
+        <is>
+          <t>Thailand</t>
+        </is>
+      </c>
+      <c r="B302" t="inlineStr">
+        <is>
+          <t>Currency: U.S. dollars</t>
+        </is>
+      </c>
+      <c r="C302" t="n">
+        <v>2012</v>
+      </c>
+      <c r="D302" t="n">
+        <v>199.916</v>
+      </c>
+    </row>
+    <row r="303">
+      <c r="A303" t="inlineStr">
+        <is>
+          <t>Thailand</t>
+        </is>
+      </c>
+      <c r="B303" t="inlineStr">
+        <is>
+          <t>Currency: U.S. dollars</t>
+        </is>
+      </c>
+      <c r="C303" t="n">
+        <v>2011</v>
+      </c>
+      <c r="D303" t="n">
+        <v>145.81</v>
+      </c>
+    </row>
+    <row r="304">
+      <c r="A304" t="inlineStr">
+        <is>
+          <t>Thailand</t>
+        </is>
+      </c>
+      <c r="B304" t="inlineStr">
+        <is>
+          <t>Currency: U.S. dollars</t>
+        </is>
+      </c>
+      <c r="C304" t="n">
+        <v>2010</v>
+      </c>
+      <c r="D304" t="n">
+        <v>131.29</v>
+      </c>
+    </row>
+    <row r="305">
+      <c r="A305" t="inlineStr">
+        <is>
+          <t>Thailand</t>
+        </is>
+      </c>
+      <c r="B305" t="inlineStr">
+        <is>
+          <t>Currency: U.S. dollars</t>
+        </is>
+      </c>
+      <c r="C305" t="n">
+        <v>2009</v>
+      </c>
+      <c r="D305" t="n">
+        <v>117.542</v>
+      </c>
+    </row>
+    <row r="306">
+      <c r="A306" t="inlineStr">
+        <is>
+          <t>Thailand</t>
+        </is>
+      </c>
+      <c r="B306" t="inlineStr">
+        <is>
+          <t>Currency: U.S. dollars</t>
+        </is>
+      </c>
+      <c r="C306" t="n">
+        <v>2008</v>
+      </c>
+      <c r="D306" t="n">
+        <v>120.973</v>
+      </c>
+    </row>
+    <row r="307">
+      <c r="A307" t="inlineStr">
+        <is>
+          <t>Thailand</t>
+        </is>
+      </c>
+      <c r="B307" t="inlineStr">
+        <is>
+          <t>Currency: U.S. dollars</t>
+        </is>
+      </c>
+      <c r="C307" t="n">
+        <v>2007</v>
+      </c>
+      <c r="D307" t="n">
+        <v>143.866</v>
+      </c>
+    </row>
+    <row r="308">
+      <c r="A308" t="inlineStr">
+        <is>
+          <t>Thailand</t>
+        </is>
+      </c>
+      <c r="B308" t="inlineStr">
+        <is>
+          <t>Currency: U.S. dollars</t>
+        </is>
+      </c>
+      <c r="C308" t="n">
+        <v>2006</v>
+      </c>
+      <c r="D308" t="n">
+        <v>126.287</v>
+      </c>
+    </row>
+    <row r="309">
+      <c r="A309" t="inlineStr">
+        <is>
+          <t>Thailand</t>
+        </is>
+      </c>
+      <c r="B309" t="inlineStr">
+        <is>
+          <t>Currency: U.S. dollars</t>
+        </is>
+      </c>
+      <c r="C309" t="n">
+        <v>2005</v>
+      </c>
+      <c r="D309" t="n">
+        <v>115.067</v>
+      </c>
+    </row>
+    <row r="310">
+      <c r="A310" t="inlineStr">
+        <is>
+          <t>Thailand</t>
+        </is>
+      </c>
+      <c r="B310" t="inlineStr">
+        <is>
+          <t>Currency: U.S. dollars</t>
+        </is>
+      </c>
+      <c r="C310" t="n">
+        <v>2004</v>
+      </c>
+      <c r="D310" t="n">
+        <v>109.889</v>
+      </c>
+    </row>
+    <row r="311">
+      <c r="A311" t="inlineStr">
+        <is>
+          <t>Thailand</t>
+        </is>
+      </c>
+      <c r="B311" t="inlineStr">
+        <is>
+          <t>Currency: U.S. dollars</t>
+        </is>
+      </c>
+      <c r="C311" t="n">
+        <v>2003</v>
+      </c>
+      <c r="D311" t="n">
+        <v>105.919</v>
+      </c>
+    </row>
+    <row r="312">
+      <c r="A312" t="inlineStr">
+        <is>
+          <t>Thailand</t>
+        </is>
+      </c>
+      <c r="B312" t="inlineStr">
+        <is>
+          <t>Currency: U.S. dollars</t>
+        </is>
+      </c>
+      <c r="C312" t="n">
+        <v>2002</v>
+      </c>
+      <c r="D312" t="n">
+        <v>99.86</v>
+      </c>
+    </row>
+    <row r="313">
+      <c r="A313" t="inlineStr">
+        <is>
+          <t>Thailand</t>
+        </is>
+      </c>
+      <c r="B313" t="inlineStr">
+        <is>
+          <t>Currency: U.S. dollars</t>
+        </is>
+      </c>
+      <c r="C313" t="n">
+        <v>2001</v>
+      </c>
+      <c r="D313" t="n">
+        <v>96.55200000000001</v>
+      </c>
+    </row>
+    <row r="314">
+      <c r="A314" t="inlineStr">
+        <is>
+          <t>Thailand</t>
+        </is>
+      </c>
+      <c r="B314" t="inlineStr">
+        <is>
+          <t>Currency: U.S. dollars</t>
+        </is>
+      </c>
+      <c r="C314" t="n">
+        <v>2000</v>
+      </c>
+      <c r="D314" t="n">
+        <v>105.006</v>
+      </c>
+    </row>
+    <row r="315">
+      <c r="A315" t="inlineStr">
+        <is>
+          <t>Thailand</t>
+        </is>
+      </c>
+      <c r="B315" t="inlineStr">
+        <is>
+          <t>Currency: U.S. dollars</t>
+        </is>
+      </c>
+      <c r="C315" t="n">
+        <v>1999</v>
+      </c>
+      <c r="D315" t="n">
+        <v>111.388</v>
+      </c>
+    </row>
+    <row r="316">
+      <c r="A316" t="inlineStr">
+        <is>
+          <t>Thailand</t>
+        </is>
+      </c>
+      <c r="B316" t="inlineStr">
+        <is>
+          <t>Currency: U.S. dollars</t>
+        </is>
+      </c>
+      <c r="C316" t="n">
+        <v>1998</v>
+      </c>
+      <c r="D316" t="n">
+        <v>101.839</v>
+      </c>
+    </row>
+    <row r="317">
+      <c r="A317" t="inlineStr">
+        <is>
+          <t>Thailand</t>
+        </is>
+      </c>
+      <c r="B317" t="inlineStr">
+        <is>
+          <t>Currency: U.S. dollars</t>
+        </is>
+      </c>
+      <c r="C317" t="n">
+        <v>1997</v>
+      </c>
+      <c r="D317" t="n">
+        <v>130.148</v>
+      </c>
+    </row>
+    <row r="318">
+      <c r="A318" t="inlineStr">
+        <is>
+          <t>Thailand</t>
+        </is>
+      </c>
+      <c r="B318" t="inlineStr">
+        <is>
+          <t>Currency: U.S. dollars</t>
+        </is>
+      </c>
+      <c r="C318" t="n">
+        <v>1996</v>
+      </c>
+      <c r="D318" t="n">
+        <v>161.072</v>
+      </c>
+    </row>
+    <row r="319">
+      <c r="A319" t="inlineStr">
+        <is>
+          <t>Thailand</t>
+        </is>
+      </c>
+      <c r="B319" t="inlineStr">
+        <is>
+          <t>Currency: U.S. dollars</t>
+        </is>
+      </c>
+      <c r="C319" t="n">
         <v>1995</v>
       </c>
-      <c r="D266" t="n">
+      <c r="D319" t="n">
         <v>151.313</v>
+      </c>
+    </row>
+    <row r="320">
+      <c r="A320" t="inlineStr">
+        <is>
+          <t>Viet Nam</t>
+        </is>
+      </c>
+      <c r="B320" t="inlineStr">
+        <is>
+          <t>Currency: U.S. dollars</t>
+        </is>
+      </c>
+      <c r="C320" t="n">
+        <v>2023</v>
+      </c>
+      <c r="D320" t="n">
+        <v>196.744</v>
+      </c>
+    </row>
+    <row r="321">
+      <c r="A321" t="inlineStr">
+        <is>
+          <t>Viet Nam</t>
+        </is>
+      </c>
+      <c r="B321" t="inlineStr">
+        <is>
+          <t>Currency: U.S. dollars</t>
+        </is>
+      </c>
+      <c r="C321" t="n">
+        <v>2022</v>
+      </c>
+      <c r="D321" t="n">
+        <v>167.396</v>
+      </c>
+    </row>
+    <row r="322">
+      <c r="A322" t="inlineStr">
+        <is>
+          <t>Viet Nam</t>
+        </is>
+      </c>
+      <c r="B322" t="inlineStr">
+        <is>
+          <t>Currency: U.S. dollars</t>
+        </is>
+      </c>
+      <c r="C322" t="n">
+        <v>2021</v>
+      </c>
+      <c r="D322" t="n">
+        <v>158.68</v>
+      </c>
+    </row>
+    <row r="323">
+      <c r="A323" t="inlineStr">
+        <is>
+          <t>Viet Nam</t>
+        </is>
+      </c>
+      <c r="B323" t="inlineStr">
+        <is>
+          <t>Currency: U.S. dollars</t>
+        </is>
+      </c>
+      <c r="C323" t="n">
+        <v>2020</v>
+      </c>
+      <c r="D323" t="n">
+        <v>158.348</v>
+      </c>
+    </row>
+    <row r="324">
+      <c r="A324" t="inlineStr">
+        <is>
+          <t>Viet Nam</t>
+        </is>
+      </c>
+      <c r="B324" t="inlineStr">
+        <is>
+          <t>Currency: U.S. dollars</t>
+        </is>
+      </c>
+      <c r="C324" t="n">
+        <v>2019</v>
+      </c>
+      <c r="D324" t="n">
+        <v>150.975</v>
+      </c>
+    </row>
+    <row r="325">
+      <c r="A325" t="inlineStr">
+        <is>
+          <t>Viet Nam</t>
+        </is>
+      </c>
+      <c r="B325" t="inlineStr">
+        <is>
+          <t>Currency: U.S. dollars</t>
+        </is>
+      </c>
+      <c r="C325" t="n">
+        <v>2018</v>
+      </c>
+      <c r="D325" t="n">
+        <v>146.447</v>
+      </c>
+    </row>
+    <row r="326">
+      <c r="A326" t="inlineStr">
+        <is>
+          <t>Viet Nam</t>
+        </is>
+      </c>
+      <c r="B326" t="inlineStr">
+        <is>
+          <t>Currency: U.S. dollars</t>
+        </is>
+      </c>
+      <c r="C326" t="n">
+        <v>2017</v>
+      </c>
+      <c r="D326" t="n">
+        <v>139.025</v>
+      </c>
+    </row>
+    <row r="327">
+      <c r="A327" t="inlineStr">
+        <is>
+          <t>Viet Nam</t>
+        </is>
+      </c>
+      <c r="B327" t="inlineStr">
+        <is>
+          <t>Currency: U.S. dollars</t>
+        </is>
+      </c>
+      <c r="C327" t="n">
+        <v>2016</v>
+      </c>
+      <c r="D327" t="n">
+        <v>132.209</v>
+      </c>
+    </row>
+    <row r="328">
+      <c r="A328" t="inlineStr">
+        <is>
+          <t>Viet Nam</t>
+        </is>
+      </c>
+      <c r="B328" t="inlineStr">
+        <is>
+          <t>Currency: U.S. dollars</t>
+        </is>
+      </c>
+      <c r="C328" t="n">
+        <v>2015</v>
+      </c>
+      <c r="D328" t="n">
+        <v>118.677</v>
+      </c>
+    </row>
+    <row r="329">
+      <c r="A329" t="inlineStr">
+        <is>
+          <t>Viet Nam</t>
+        </is>
+      </c>
+      <c r="B329" t="inlineStr">
+        <is>
+          <t>Currency: U.S. dollars</t>
+        </is>
+      </c>
+      <c r="C329" t="n">
+        <v>2014</v>
+      </c>
+      <c r="D329" t="n">
+        <v>106.393</v>
+      </c>
+    </row>
+    <row r="330">
+      <c r="A330" t="inlineStr">
+        <is>
+          <t>Viet Nam</t>
+        </is>
+      </c>
+      <c r="B330" t="inlineStr">
+        <is>
+          <t>Currency: U.S. dollars</t>
+        </is>
+      </c>
+      <c r="C330" t="n">
+        <v>2013</v>
+      </c>
+      <c r="D330" t="n">
+        <v>93.152</v>
+      </c>
+    </row>
+    <row r="331">
+      <c r="A331" t="inlineStr">
+        <is>
+          <t>Viet Nam</t>
+        </is>
+      </c>
+      <c r="B331" t="inlineStr">
+        <is>
+          <t>Currency: U.S. dollars</t>
+        </is>
+      </c>
+      <c r="C331" t="n">
+        <v>2012</v>
+      </c>
+      <c r="D331" t="n">
+        <v>79.94</v>
+      </c>
+    </row>
+    <row r="332">
+      <c r="A332" t="inlineStr">
+        <is>
+          <t>Viet Nam</t>
+        </is>
+      </c>
+      <c r="B332" t="inlineStr">
+        <is>
+          <t>Currency: U.S. dollars</t>
+        </is>
+      </c>
+      <c r="C332" t="n">
+        <v>2011</v>
+      </c>
+      <c r="D332" t="n">
+        <v>54.852</v>
+      </c>
+    </row>
+    <row r="333">
+      <c r="A333" t="inlineStr">
+        <is>
+          <t>Viet Nam</t>
+        </is>
+      </c>
+      <c r="B333" t="inlineStr">
+        <is>
+          <t>Currency: U.S. dollars</t>
+        </is>
+      </c>
+      <c r="C333" t="n">
+        <v>2010</v>
+      </c>
+      <c r="D333" t="n">
+        <v>45.399</v>
+      </c>
+    </row>
+    <row r="334">
+      <c r="A334" t="inlineStr">
+        <is>
+          <t>Viet Nam</t>
+        </is>
+      </c>
+      <c r="B334" t="inlineStr">
+        <is>
+          <t>Currency: U.S. dollars</t>
+        </is>
+      </c>
+      <c r="C334" t="n">
+        <v>2009</v>
+      </c>
+      <c r="D334" t="n">
+        <v>38.09</v>
+      </c>
+    </row>
+    <row r="335">
+      <c r="A335" t="inlineStr">
+        <is>
+          <t>Viet Nam</t>
+        </is>
+      </c>
+      <c r="B335" t="inlineStr">
+        <is>
+          <t>Currency: U.S. dollars</t>
+        </is>
+      </c>
+      <c r="C335" t="n">
+        <v>2008</v>
+      </c>
+      <c r="D335" t="n">
+        <v>33.124</v>
+      </c>
+    </row>
+    <row r="336">
+      <c r="A336" t="inlineStr">
+        <is>
+          <t>Viet Nam</t>
+        </is>
+      </c>
+      <c r="B336" t="inlineStr">
+        <is>
+          <t>Currency: U.S. dollars</t>
+        </is>
+      </c>
+      <c r="C336" t="n">
+        <v>2007</v>
+      </c>
+      <c r="D336" t="n">
+        <v>33.53</v>
+      </c>
+    </row>
+    <row r="337">
+      <c r="A337" t="inlineStr">
+        <is>
+          <t>Viet Nam</t>
+        </is>
+      </c>
+      <c r="B337" t="inlineStr">
+        <is>
+          <t>Currency: U.S. dollars</t>
+        </is>
+      </c>
+      <c r="C337" t="n">
+        <v>2006</v>
+      </c>
+      <c r="D337" t="n">
+        <v>28.135</v>
+      </c>
+    </row>
+    <row r="338">
+      <c r="A338" t="inlineStr">
+        <is>
+          <t>Viet Nam</t>
+        </is>
+      </c>
+      <c r="B338" t="inlineStr">
+        <is>
+          <t>Currency: U.S. dollars</t>
+        </is>
+      </c>
+      <c r="C338" t="n">
+        <v>2005</v>
+      </c>
+      <c r="D338" t="n">
+        <v>22.07</v>
+      </c>
+    </row>
+    <row r="339">
+      <c r="A339" t="inlineStr">
+        <is>
+          <t>Viet Nam</t>
+        </is>
+      </c>
+      <c r="B339" t="inlineStr">
+        <is>
+          <t>Currency: U.S. dollars</t>
+        </is>
+      </c>
+      <c r="C339" t="n">
+        <v>2004</v>
+      </c>
+      <c r="D339" t="n">
+        <v>18.417</v>
+      </c>
+    </row>
+    <row r="340">
+      <c r="A340" t="inlineStr">
+        <is>
+          <t>Viet Nam</t>
+        </is>
+      </c>
+      <c r="B340" t="inlineStr">
+        <is>
+          <t>Currency: U.S. dollars</t>
+        </is>
+      </c>
+      <c r="C340" t="n">
+        <v>2003</v>
+      </c>
+      <c r="D340" t="n">
+        <v>18.698</v>
+      </c>
+    </row>
+    <row r="341">
+      <c r="A341" t="inlineStr">
+        <is>
+          <t>Viet Nam</t>
+        </is>
+      </c>
+      <c r="B341" t="inlineStr">
+        <is>
+          <t>Currency: U.S. dollars</t>
+        </is>
+      </c>
+      <c r="C341" t="n">
+        <v>2002</v>
+      </c>
+      <c r="D341" t="n">
+        <v>13.744</v>
+      </c>
+    </row>
+    <row r="342">
+      <c r="A342" t="inlineStr">
+        <is>
+          <t>Viet Nam</t>
+        </is>
+      </c>
+      <c r="B342" t="inlineStr">
+        <is>
+          <t>Currency: U.S. dollars</t>
+        </is>
+      </c>
+      <c r="C342" t="n">
+        <v>2001</v>
+      </c>
+      <c r="D342" t="n">
+        <v>12.224</v>
+      </c>
+    </row>
+    <row r="343">
+      <c r="A343" t="inlineStr">
+        <is>
+          <t>Viet Nam</t>
+        </is>
+      </c>
+      <c r="B343" t="inlineStr">
+        <is>
+          <t>Currency: U.S. dollars</t>
+        </is>
+      </c>
+      <c r="C343" t="n">
+        <v>2000</v>
+      </c>
+      <c r="D343" t="n">
+        <v>12.705</v>
       </c>
     </row>
   </sheetData>

</xml_diff>